<commit_message>
Modify database and Demo
</commit_message>
<xml_diff>
--- a/dev/Demo.xlsx
+++ b/dev/Demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fy386\Desktop\Database\Project\DatabaseProject_server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fy386\Desktop\Database\Project\DatabaseProject_server\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C393D1-74C4-451D-93FA-135D9A659B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B96FE1F-8EF1-4D2D-93D8-BAC6B5A27BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USERS" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="118">
   <si>
     <t>UID</t>
   </si>
@@ -204,10 +204,6 @@
     </r>
   </si>
   <si>
-    <t>int. 喂；哈罗
-n. 表示问候， 惊奇或唤起注意时的用语</t>
-  </si>
-  <si>
     <t>需要考虑如何把不同的意思、词性分开</t>
   </si>
   <si>
@@ -456,9 +452,6 @@
     <t>int[]</t>
   </si>
   <si>
-    <t>numeric[]</t>
-  </si>
-  <si>
     <t>{10 0 0 0}</t>
   </si>
   <si>
@@ -508,9 +501,6 @@
   </si>
   <si>
     <t>Info</t>
-  </si>
-  <si>
-    <t>varchar</t>
   </si>
   <si>
     <t>2019-12-27-00-01-20</t>
@@ -538,6 +528,66 @@
   <si>
     <t>int</t>
     <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>dates</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>020-01-02</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-01-04</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-01-05</t>
+  </si>
+  <si>
+    <t>2020-01-03</t>
+  </si>
+  <si>
+    <t>text</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>float[]</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>int. 喂；哈罗
+n. 表示问候， 惊奇或唤起注意时的用语</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -547,7 +597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +656,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -677,7 +735,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
@@ -698,6 +756,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="标题 1" xfId="3" builtinId="16"/>
@@ -1162,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1205,7 +1267,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>14</v>
@@ -1222,11 +1284,11 @@
       <c r="C3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1234,13 +1296,13 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1248,41 +1310,41 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>49</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1308,19 +1370,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1345,16 +1407,16 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D3">
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1362,16 +1424,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="D4">
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1379,21 +1441,21 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1417,10 +1479,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>34</v>
@@ -1456,7 +1518,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1467,12 +1529,12 @@
         <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
@@ -1483,7 +1545,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>27</v>
@@ -1503,12 +1565,13 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.4">
@@ -1516,16 +1579,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1535,14 +1598,14 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="E2" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1552,11 +1615,11 @@
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1566,11 +1629,11 @@
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1578,13 +1641,13 @@
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>99</v>
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1592,13 +1655,13 @@
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>99</v>
+        <v>54</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1608,16 +1671,17 @@
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7">
-        <v>23</v>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1625,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1639,28 +1703,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
@@ -1671,19 +1735,19 @@
         <v>9</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>13</v>
@@ -1706,10 +1770,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1732,10 +1796,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1758,10 +1822,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1769,7 +1833,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>15</v>
@@ -1784,10 +1848,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -1795,7 +1859,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>22</v>
@@ -1810,10 +1874,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1821,7 +1885,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>27</v>
@@ -1836,10 +1900,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -1847,12 +1911,12 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G9" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G10" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1867,23 +1931,23 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1894,10 +1958,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1908,10 +1972,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1922,10 +1986,10 @@
         <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1933,7 +1997,7 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>